<commit_message>
Import gpx signalisation et creation shapefile signalisation, ref #30
- Création fichier gpx pour Etape 1 (pas complet) et modification fichier excel signalisation.xlsx en conséquence
- Modification des colonnes au fichier signalisation.xlsx
- Création d'un script d'importation des données de signalisation des GPX et excel : _importExportGPX_Signalisation.R
- Création des shapefiles `points_signalisation.shp` contenant toute l'information (points geometry et df) sur les signalisation de toutes les étapes, pouvant être lu par les prochaines étapes
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Documents\guide2023\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC62BBBE-6E3D-45B8-82F6-4C309E8699DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF500649-CC9C-A246-814B-85BAFA7CBB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32475" windowHeight="21000" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14060" yWindow="4440" windowWidth="32480" windowHeight="21000" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
     <sheet name="Lexique" sheetId="20" r:id="rId2"/>
-    <sheet name="Etape1" sheetId="26" r:id="rId3"/>
-    <sheet name="Etape1_CSV" sheetId="25" r:id="rId4"/>
+    <sheet name="Etape1" sheetId="27" r:id="rId3"/>
+    <sheet name="Etape2" sheetId="26" r:id="rId4"/>
+    <sheet name="Etape1_CSV" sheetId="28" r:id="rId5"/>
+    <sheet name="Etape2_CSV" sheetId="25" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -69,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="152">
   <si>
     <t>GPM</t>
   </si>
@@ -98,9 +100,6 @@
     <t>Déviation droite</t>
   </si>
   <si>
-    <t>Symbol</t>
-  </si>
-  <si>
     <t>Dernier passage</t>
   </si>
   <si>
@@ -239,9 +238,6 @@
     <t>id</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
     <t>symbol</t>
   </si>
   <si>
@@ -278,9 +274,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>virage</t>
-  </si>
-  <si>
     <t>section_gravier</t>
   </si>
   <si>
@@ -320,15 +313,6 @@
     <t>Terre-plein, entrée giratoire Saguenay</t>
   </si>
   <si>
-    <t>Pour un terre-plein : Signal(cue) perso à Danger - terre_plein dans description // POI est mise en garde</t>
-  </si>
-  <si>
-    <t>Pour un virage : Signal(cue) perso à Control - virage dans description // POI est contrôle</t>
-  </si>
-  <si>
-    <t>Pour du gravier : Signal(cue) perso à xxx - section_gravier dans description // POI est xxx</t>
-  </si>
-  <si>
     <t>Entrée pont de bois Mont-Brun</t>
   </si>
   <si>
@@ -377,24 +361,12 @@
     <t>Gestion de ligne / zone décélération</t>
   </si>
   <si>
-    <t>Pour voir apparaître les indications au fihcier CSV, il faut mettre les détails en cue (signal perso)</t>
-  </si>
-  <si>
     <t>Pour voir apparaître les icônes sur la carte, il faut ajouter les POI</t>
   </si>
   <si>
-    <t>Details_FR</t>
-  </si>
-  <si>
     <t>KM_reel</t>
   </si>
   <si>
-    <t>Sharp Right</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
     <t>Start of route</t>
   </si>
   <si>
@@ -506,16 +478,55 @@
     <t>End of route</t>
   </si>
   <si>
-    <t>control</t>
-  </si>
-  <si>
-    <t>intersection</t>
-  </si>
-  <si>
     <t>sign_17</t>
   </si>
   <si>
-    <t>Description</t>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>Terre-plein 8e rue &amp; Blvd Lamaque</t>
+  </si>
+  <si>
+    <t>Virage à droite et terre-plein sur le 7e rue</t>
+  </si>
+  <si>
+    <t>Entrée carrefour giratoire 7e rue &amp; 117, tout à droite</t>
+  </si>
+  <si>
+    <t>Terre-plein intersection 7e &amp; 7e (tout droit)</t>
+  </si>
+  <si>
+    <t>Terre-plein blvd JJ Cossette (tout à droite, devant cours à bois Eacom)</t>
+  </si>
+  <si>
+    <t>Terre-plein blvd JJ Cossette (tout à droite, devant Orbit Garant)</t>
+  </si>
+  <si>
+    <t>Terre-plein blvd JJ Cossette (tout à droite, avant du Portage)</t>
+  </si>
+  <si>
+    <t>Terre-plein blvd JJ Cossette (tout à droite, intersection du Portage)</t>
+  </si>
+  <si>
+    <t>Pour voir apparaître les indications au fichier CSV, il faut mettre les détails en cue (signal perso)</t>
+  </si>
+  <si>
+    <t>Pour un terre-plein : Signal(cue) perso à Danger - terre_plein dans description // POI est Caution</t>
+  </si>
+  <si>
+    <t>Pour un virage : Signal(cue) perso à Control - virage dans description // POI est Control</t>
+  </si>
+  <si>
+    <t>Pour du gravier/ voie ferrée : Signal(cue) perso à Danger - section_gravier dans description // POI est Danger</t>
+  </si>
+  <si>
+    <t>details</t>
+  </si>
+  <si>
+    <t>Besoin de copier le csv des cues pour obtenir les distances : distances et notes (qui réfèrent à sign_xx)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans RWGPS, le nom doit toujours être sign_xx pour le Cue et le POI, pour le référencer après. </t>
   </si>
 </sst>
 </file>
@@ -524,9 +535,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0#"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -572,6 +583,22 @@
       <b/>
       <sz val="9"/>
       <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Trebuchet MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -645,7 +672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -659,8 +686,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -865,7 +897,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Bureau">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -903,7 +935,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Bureau">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1009,7 +1041,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Bureau">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1183,55 +1215,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AF60EC-7F0F-4893-B669-95F24DB4647E}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="88.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>85</v>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A9" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="13" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1248,283 +1290,283 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16.875" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1541,57 +1583,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4800E175-391C-4882-AD71-91732BA4C7F2}">
-  <dimension ref="A1:I18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59035EEC-8A2E-CE47-A69A-0CAB24334359}">
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.75" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="62.5" customWidth="1"/>
-    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>67</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -1601,28 +1640,24 @@
         <v>sign_01</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H2" t="str">
-        <f>_xlfn.CONCAT(A2,"/sign_",B2,".png")</f>
-        <v>E1/sign_1.png</v>
-      </c>
-      <c r="I2" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C2,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="str">
+        <v>59</v>
+      </c>
+      <c r="H2" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C2,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="10" t="str">
         <f>A2</f>
         <v>E1</v>
       </c>
@@ -1630,33 +1665,29 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f t="shared" ref="C3:C18" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <f t="shared" ref="C3:C10" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
         <v>sign_02</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H18" si="1">_xlfn.CONCAT(A3,"/sign_",B3,".png")</f>
-        <v>E1/sign_2.png</v>
-      </c>
-      <c r="I3" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C3,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="str">
-        <f t="shared" ref="A4:A18" si="2">A3</f>
+        <v>59</v>
+      </c>
+      <c r="H3" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C3,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="10" t="str">
+        <f t="shared" ref="A4:A5" si="1">A3</f>
         <v>E1</v>
       </c>
       <c r="B4" s="5">
@@ -1667,194 +1698,170 @@
         <v>sign_03</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" t="str">
+        <v>59</v>
+      </c>
+      <c r="H4" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C4,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>E1/sign_3.png</v>
-      </c>
-      <c r="I4" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C4,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
-        <f>A9</f>
         <v>E1</v>
       </c>
       <c r="B5" s="5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5" s="5" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B5,"0#"))</f>
-        <v>sign_08</v>
+        <f t="shared" si="0"/>
+        <v>sign_04</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="G5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" t="str">
-        <f>_xlfn.CONCAT(A5,"/sign_",B5,".png")</f>
-        <v>E1/sign_8.png</v>
-      </c>
-      <c r="I5" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C5,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="str">
-        <f>A4</f>
+        <v>59</v>
+      </c>
+      <c r="H5" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C5,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="10" t="str">
+        <f t="shared" ref="A6:A10" si="2">A5</f>
         <v>E1</v>
       </c>
       <c r="B6" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>sign_04</v>
+        <v>sign_05</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_4.png</v>
-      </c>
-      <c r="I6" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C6,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="str">
+        <v>72</v>
+      </c>
+      <c r="H6" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C6,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="10" t="str">
         <f t="shared" si="2"/>
         <v>E1</v>
       </c>
       <c r="B7" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>sign_05</v>
+        <v>sign_06</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>141</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_5.png</v>
-      </c>
-      <c r="I7" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C7,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>33.799999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="str">
+        <v>59</v>
+      </c>
+      <c r="H7" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C7,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="10" t="str">
         <f t="shared" si="2"/>
         <v>E1</v>
       </c>
       <c r="B8" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>sign_06</v>
+        <v>sign_07</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_6.png</v>
-      </c>
-      <c r="I8" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C8,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>46.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="str">
+        <v>59</v>
+      </c>
+      <c r="H8" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C8,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="10" t="str">
         <f t="shared" si="2"/>
         <v>E1</v>
       </c>
       <c r="B9" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>sign_07</v>
+        <v>sign_08</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_7.png</v>
-      </c>
-      <c r="I9" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C9,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>54.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="str">
-        <f>A5</f>
+        <v>59</v>
+      </c>
+      <c r="H9" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C9,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" s="10" t="str">
+        <f t="shared" si="2"/>
         <v>E1</v>
       </c>
       <c r="B10" s="5">
@@ -1865,793 +1872,1065 @@
         <v>sign_09</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_9.png</v>
-      </c>
-      <c r="I10" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C10,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>75.099999999999994</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="str">
-        <f t="shared" si="2"/>
-        <v>E1</v>
-      </c>
-      <c r="B11" s="5">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_10</v>
-      </c>
-      <c r="D11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" t="s">
-        <v>87</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_10.png</v>
-      </c>
-      <c r="I11" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C11,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>77.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="str">
-        <f t="shared" si="2"/>
-        <v>E1</v>
-      </c>
-      <c r="B12" s="5">
-        <v>11</v>
-      </c>
-      <c r="C12" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_11.png</v>
-      </c>
-      <c r="I12" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C12,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>87.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="str">
-        <f t="shared" si="2"/>
-        <v>E1</v>
-      </c>
-      <c r="B13" s="5">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F13" t="s">
-        <v>98</v>
-      </c>
-      <c r="G13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_12.png</v>
-      </c>
-      <c r="I13" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C13,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>89.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="str">
-        <f t="shared" si="2"/>
-        <v>E1</v>
-      </c>
-      <c r="B14" s="5">
-        <v>13</v>
-      </c>
-      <c r="C14" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" t="s">
-        <v>96</v>
-      </c>
-      <c r="G14" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_13.png</v>
-      </c>
-      <c r="I14" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C14,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>112.7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="str">
-        <f t="shared" si="2"/>
-        <v>E1</v>
-      </c>
-      <c r="B15" s="5">
-        <v>14</v>
-      </c>
-      <c r="C15" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_14</v>
-      </c>
-      <c r="D15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" t="s">
-        <v>98</v>
-      </c>
-      <c r="G15" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_14.png</v>
-      </c>
-      <c r="I15" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C15,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>134.80000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="str">
-        <f t="shared" si="2"/>
-        <v>E1</v>
-      </c>
-      <c r="B16" s="5">
-        <v>15</v>
-      </c>
-      <c r="C16" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" t="s">
-        <v>76</v>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_15.png</v>
-      </c>
-      <c r="I16" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C16,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>135.30000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="str">
-        <f t="shared" si="2"/>
-        <v>E1</v>
-      </c>
-      <c r="B17" s="5">
-        <v>16</v>
-      </c>
-      <c r="C17" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_16.png</v>
-      </c>
-      <c r="I17" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C17,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>135.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="str">
-        <f t="shared" si="2"/>
-        <v>E1</v>
-      </c>
-      <c r="B18" s="5">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" t="s">
-        <v>96</v>
-      </c>
-      <c r="G18" t="s">
-        <v>76</v>
-      </c>
-      <c r="H18" t="str">
-        <f t="shared" si="1"/>
-        <v>E1/sign_17.png</v>
-      </c>
-      <c r="I18" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C18,Etape1_CSV!$C$2:$C$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>136.69999999999999</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="H10" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C10,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" s="10"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="10"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="10"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="10"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" s="10"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="10"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="10"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="10"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="H18" s="9"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D5E8AE-63D3-48B9-85FC-50E5B76DED54}">
-  <dimension ref="A1:D39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4800E175-391C-4882-AD71-91732BA4C7F2}">
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <v>sign_01</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C2,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>A2</f>
+        <v>E2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f t="shared" ref="C3:C18" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <v>sign_02</v>
+      </c>
+      <c r="D3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C3,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A18" si="1">A3</f>
+        <v>E2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_03</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C4,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" t="str">
+        <f>A9</f>
+        <v>E2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B5,"0#"))</f>
+        <v>sign_08</v>
+      </c>
+      <c r="D5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C5,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" t="str">
+        <f>A4</f>
+        <v>E2</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_04</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C6,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B7" s="5">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_05</v>
+      </c>
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C7,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B8" s="5">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_06</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C8,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>46.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B9" s="5">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_07</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C9,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>54.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A10" t="str">
+        <f>A5</f>
+        <v>E2</v>
+      </c>
+      <c r="B10" s="5">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_09</v>
+      </c>
+      <c r="D10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H10" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C10,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>75.099999999999994</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A11" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B11" s="5">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C11,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B12" s="5">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C12,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>87.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B13" s="5">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C13,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>89.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B14" s="5">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C14,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>112.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A15" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B15" s="5">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C15,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>134.80000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B16" s="5">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C16,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>135.30000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B17" s="5">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C17,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>135.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" t="str">
+        <f t="shared" si="1"/>
+        <v>E2</v>
+      </c>
+      <c r="B18" s="5">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="9">
+        <f>ROUND(_xlfn.XLOOKUP(C18,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
+        <v>136.69999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{207A86C0-F1FC-5647-BA0D-4DE47D82F8C4}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.15">
+      <c r="A1" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="12">
+        <v>0</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="12">
+        <v>0.98</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="12">
+        <v>1.04</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="12">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="12">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="12">
+        <v>2.48</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="12">
+        <v>2.57</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="12">
+        <v>119.44</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D5E8AE-63D3-48B9-85FC-50E5B76DED54}">
+  <dimension ref="A1:B39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>0.16</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>0.86</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>0.96</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2.68</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>4.04</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>4.04</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8.82</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>8.98</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>33.82</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>44.88</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>46.16</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>46.18</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>54.64</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>126</v>
-      </c>
-      <c r="D20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>75.099999999999994</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>77.459999999999994</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>128</v>
-      </c>
-      <c r="D22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>87.8</v>
       </c>
       <c r="B23" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>87.8</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" t="s">
-        <v>130</v>
-      </c>
-      <c r="D24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>89.05</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>89.23</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
-      </c>
-      <c r="C26" t="s">
-        <v>132</v>
-      </c>
-      <c r="D26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>89.24</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>112.65</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>134.77000000000001</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>134.77000000000001</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30" t="s">
-        <v>136</v>
-      </c>
-      <c r="D30" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>135.27000000000001</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" t="s">
-        <v>137</v>
-      </c>
-      <c r="D31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>135.44999999999999</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C32" t="s">
-        <v>138</v>
-      </c>
-      <c r="D32" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>135.46</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>135.56</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>135.79</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
-      </c>
-      <c r="C35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>136.19</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>136.37</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
-      </c>
-      <c r="C37" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>136.69999999999999</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" t="s">
-        <v>147</v>
-      </c>
-      <c r="D38" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>136.71</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Création structure pour guide organisateur, ref #31
- Création du git_book_organisateur pour le site d'organisation
- Sélection des fichiers .Rmd existant à ajouter au site organisation
- Modification du snakefile et du .gitignore
- Ajout de la partie Signalisation à ajouter pour chaque étape, avec ajout de la photo, localisation sur la carte de détails (vignette) et quelques points d'information
- Ajout d'un tableau résumé par étape avec tous les POIs de signalisation
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF500649-CC9C-A246-814B-85BAFA7CBB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D018B280-3B4A-9C46-BA40-FCEB3E006976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="4440" windowWidth="32480" windowHeight="21000" tabRatio="758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68920" yWindow="6780" windowWidth="32480" windowHeight="21000" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -50,7 +50,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Bruno Gauthier:</t>
         </r>
@@ -59,7 +59,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 à entrer dans description du signal personnalisé RWG, pour jointure</t>
@@ -484,18 +484,6 @@
     <t>E2</t>
   </si>
   <si>
-    <t>Terre-plein 8e rue &amp; Blvd Lamaque</t>
-  </si>
-  <si>
-    <t>Virage à droite et terre-plein sur le 7e rue</t>
-  </si>
-  <si>
-    <t>Entrée carrefour giratoire 7e rue &amp; 117, tout à droite</t>
-  </si>
-  <si>
-    <t>Terre-plein intersection 7e &amp; 7e (tout droit)</t>
-  </si>
-  <si>
     <t>Terre-plein blvd JJ Cossette (tout à droite, devant cours à bois Eacom)</t>
   </si>
   <si>
@@ -527,6 +515,18 @@
   </si>
   <si>
     <t xml:space="preserve">Dans RWGPS, le nom doit toujours être sign_xx pour le Cue et le POI, pour le référencer après. </t>
+  </si>
+  <si>
+    <t>Terre-plein 8e rue &amp; Blvd Lamaque (tout à droite)</t>
+  </si>
+  <si>
+    <t>Virage à droite et terre-plein sur la 7e rue (tout à droite)</t>
+  </si>
+  <si>
+    <t>Terre-plein intersection 7e &amp; 7e (tout à droite)</t>
+  </si>
+  <si>
+    <t>Entrée carrefour giratoire 7e rue &amp; 117, (tout à droite)</t>
   </si>
 </sst>
 </file>
@@ -570,14 +570,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -588,6 +588,7 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -672,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -692,7 +693,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1217,7 +1217,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AF60EC-7F0F-4893-B669-95F24DB4647E}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
@@ -1253,27 +1253,27 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="13" t="s">
-        <v>151</v>
+      <c r="A9" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
-        <v>150</v>
+      <c r="A10" s="2" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1287,7 +1287,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1405,7 +1405,7 @@
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1586,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59035EEC-8A2E-CE47-A69A-0CAB24334359}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1613,7 +1613,7 @@
         <v>65</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>68</v>
@@ -1639,8 +1639,8 @@
         <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
         <v>sign_01</v>
       </c>
-      <c r="D2" t="s">
-        <v>137</v>
+      <c r="D2" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="E2" t="s">
         <v>70</v>
@@ -1668,8 +1668,8 @@
         <f t="shared" ref="C3:C10" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
         <v>sign_02</v>
       </c>
-      <c r="D3" t="s">
-        <v>138</v>
+      <c r="D3" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="E3" t="s">
         <v>70</v>
@@ -1697,8 +1697,8 @@
         <f t="shared" si="0"/>
         <v>sign_03</v>
       </c>
-      <c r="D4" t="s">
-        <v>140</v>
+      <c r="D4" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="E4" t="s">
         <v>70</v>
@@ -1726,8 +1726,8 @@
         <f t="shared" si="0"/>
         <v>sign_04</v>
       </c>
-      <c r="D5" t="s">
-        <v>139</v>
+      <c r="D5" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="E5" t="s">
         <v>70</v>
@@ -1785,7 +1785,7 @@
         <v>sign_06</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E7" t="s">
         <v>70</v>
@@ -1814,7 +1814,7 @@
         <v>sign_07</v>
       </c>
       <c r="D8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
         <v>70</v>
@@ -1843,7 +1843,7 @@
         <v>sign_08</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E9" t="s">
         <v>70</v>
@@ -1872,7 +1872,7 @@
         <v>sign_09</v>
       </c>
       <c r="D10" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E10" t="s">
         <v>70</v>
@@ -1974,7 +1974,7 @@
         <v>65</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Modification fonction pour joindre les km POIs signalisation à partie du fichier csv ,closes #33
- code/_importExportGPX_Signalisation.R modifié pour faire un left_join avec le fichier csv et le fichier excel de signalisation
- correction du fichier excel signalisation et préparation onglets pour autres étapes
- ajout des fichiers csv (cuesheet de RWGPS) pour étape 1 et 2
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D018B280-3B4A-9C46-BA40-FCEB3E006976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06EB223-400B-8F4F-A78D-356185FFFD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68920" yWindow="6780" windowWidth="32480" windowHeight="21000" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36540" yWindow="3780" windowWidth="32480" windowHeight="21000" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
     <sheet name="Lexique" sheetId="20" r:id="rId2"/>
     <sheet name="Etape1" sheetId="27" r:id="rId3"/>
     <sheet name="Etape2" sheetId="26" r:id="rId4"/>
-    <sheet name="Etape1_CSV" sheetId="28" r:id="rId5"/>
-    <sheet name="Etape2_CSV" sheetId="25" r:id="rId6"/>
+    <sheet name="Etape3" sheetId="31" r:id="rId5"/>
+    <sheet name="Etape4" sheetId="32" r:id="rId6"/>
+    <sheet name="Etape5" sheetId="33" r:id="rId7"/>
+    <sheet name="Etape6" sheetId="34" r:id="rId8"/>
+    <sheet name="Etape7" sheetId="35" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -71,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="117">
   <si>
     <t>GPM</t>
   </si>
@@ -115,9 +118,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Utiliser '&lt;br/&gt;' pour indiquer un saut de ligne dans le tableau des détails</t>
-  </si>
-  <si>
     <t>Départ neutralisé</t>
   </si>
   <si>
@@ -364,123 +364,6 @@
     <t>Pour voir apparaître les icônes sur la carte, il faut ajouter les POI</t>
   </si>
   <si>
-    <t>KM_reel</t>
-  </si>
-  <si>
-    <t>Start of route</t>
-  </si>
-  <si>
-    <t>Tournez Ã  droite sur Boulevard du CollÃ¨ge</t>
-  </si>
-  <si>
-    <t>sign_01</t>
-  </si>
-  <si>
-    <t>Tournez Ã  gauche sur Rue Tardif</t>
-  </si>
-  <si>
-    <t>Tournez Ã  gauche sur Avenue LalibertÃ©</t>
-  </si>
-  <si>
-    <t>Tournez Ã  droite sur Rue Marie-Victorin</t>
-  </si>
-  <si>
-    <t>Tournez Ã  droite sur Rue Perreault Est</t>
-  </si>
-  <si>
-    <t>Tournez Ã  gauche sur 117 - Voie de contournement, 117</t>
-  </si>
-  <si>
-    <t>sign_02</t>
-  </si>
-  <si>
-    <t>sign_03</t>
-  </si>
-  <si>
-    <t>sign_08</t>
-  </si>
-  <si>
-    <t>Restez sur la droite sur Rue du Saguenay, 101</t>
-  </si>
-  <si>
-    <t>Tournez Ã  droite sur Route D'Aiguebelle</t>
-  </si>
-  <si>
-    <t>sign_04</t>
-  </si>
-  <si>
-    <t>sign_05</t>
-  </si>
-  <si>
-    <t>Tournez Ã  gauche sur Route D'Aiguebelle</t>
-  </si>
-  <si>
-    <t>Tournez Ã  droite sur Rue Principale</t>
-  </si>
-  <si>
-    <t>sign_06</t>
-  </si>
-  <si>
-    <t>sign_07</t>
-  </si>
-  <si>
-    <t>sign_09</t>
-  </si>
-  <si>
-    <t>sign_10</t>
-  </si>
-  <si>
-    <t>Tournez fort Ã  droite sur Chemin des Pionniers, 390</t>
-  </si>
-  <si>
-    <t>sign_11</t>
-  </si>
-  <si>
-    <t>Tournez Ã  gauche sur Rue Principale, 390</t>
-  </si>
-  <si>
-    <t>sign_12</t>
-  </si>
-  <si>
-    <t>Tournez Ã  droite sur Avenue Privat, 111</t>
-  </si>
-  <si>
-    <t>sign_13</t>
-  </si>
-  <si>
-    <t>Continuez sur 1re Avenue Ouest</t>
-  </si>
-  <si>
-    <t>sign_14</t>
-  </si>
-  <si>
-    <t>sign_15</t>
-  </si>
-  <si>
-    <t>sign_16</t>
-  </si>
-  <si>
-    <t>Tournez Ã  gauche sur Boulevard Mercier</t>
-  </si>
-  <si>
-    <t>Tournez Ã  droite sur 2e Avenue Ouest</t>
-  </si>
-  <si>
-    <t>Tournez Ã  gauche sur 1re Rue Ouest</t>
-  </si>
-  <si>
-    <t>Tournez Ã  droite sur 5e Avenue Ouest</t>
-  </si>
-  <si>
-    <t>Tournez Ã  droite sur Rue Principale Nord</t>
-  </si>
-  <si>
-    <t>End of route</t>
-  </si>
-  <si>
-    <t>sign_17</t>
-  </si>
-  <si>
     <t>E2</t>
   </si>
   <si>
@@ -511,9 +394,6 @@
     <t>details</t>
   </si>
   <si>
-    <t>Besoin de copier le csv des cues pour obtenir les distances : distances et notes (qui réfèrent à sign_xx)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dans RWGPS, le nom doit toujours être sign_xx pour le Cue et le POI, pour le référencer après. </t>
   </si>
   <si>
@@ -527,17 +407,34 @@
   </si>
   <si>
     <t>Entrée carrefour giratoire 7e rue &amp; 117, (tout à droite)</t>
+  </si>
+  <si>
+    <t>sq_autre</t>
+  </si>
+  <si>
+    <t>Utiliser '&lt;br/&gt;' pour forcer un saut de ligne dans le tableau des détails</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>Description 1</t>
+  </si>
+  <si>
+    <t>-------------------</t>
+  </si>
+  <si>
+    <t>Besoin d'importer le GPX avec POI et le fichier CSV pour bon fonctionnement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0#"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -580,30 +477,12 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,24 +496,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE6E6E6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -653,27 +520,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -682,17 +534,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1215,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3AF60EC-7F0F-4893-B669-95F24DB4647E}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1233,47 +1079,52 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>141</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>142</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>143</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>144</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>147</v>
+      <c r="A9" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>146</v>
+      <c r="A10" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1287,7 +1138,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1300,99 +1151,99 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -1400,13 +1251,13 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -1414,46 +1265,49 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="F9" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -1461,10 +1315,10 @@
     </row>
     <row r="11" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
@@ -1472,32 +1326,32 @@
     </row>
     <row r="12" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
@@ -1505,10 +1359,10 @@
     </row>
     <row r="15" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>8</v>
@@ -1516,10 +1370,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>10</v>
@@ -1527,10 +1381,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>11</v>
@@ -1538,35 +1392,35 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
         <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1584,10 +1438,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59035EEC-8A2E-CE47-A69A-0CAB24334359}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1599,38 +1453,34 @@
     <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
-        <v>64</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -1640,24 +1490,20 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C2,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="8" t="str">
         <f>A2</f>
         <v>E1</v>
       </c>
@@ -1669,24 +1515,20 @@
         <v>sign_02</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C3,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="10" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="str">
         <f t="shared" ref="A4:A5" si="1">A3</f>
         <v>E1</v>
       </c>
@@ -1698,24 +1540,20 @@
         <v>sign_03</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>150</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C4,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="10" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="str">
         <f t="shared" si="1"/>
         <v>E1</v>
       </c>
@@ -1727,24 +1565,20 @@
         <v>sign_04</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C5,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A6" s="10" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="str">
         <f t="shared" ref="A6:A10" si="2">A5</f>
         <v>E1</v>
       </c>
@@ -1756,24 +1590,20 @@
         <v>sign_05</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C6,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="10" t="str">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="8" t="str">
         <f t="shared" si="2"/>
         <v>E1</v>
       </c>
@@ -1785,24 +1615,20 @@
         <v>sign_06</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C7,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="10" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="8" t="str">
         <f t="shared" si="2"/>
         <v>E1</v>
       </c>
@@ -1814,24 +1640,20 @@
         <v>sign_07</v>
       </c>
       <c r="D8" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C8,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="10" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="str">
         <f t="shared" si="2"/>
         <v>E1</v>
       </c>
@@ -1843,24 +1665,20 @@
         <v>sign_08</v>
       </c>
       <c r="D9" t="s">
-        <v>139</v>
+        <v>99</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H9" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C9,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="10" t="str">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="str">
         <f t="shared" si="2"/>
         <v>E1</v>
       </c>
@@ -1872,83 +1690,95 @@
         <v>sign_09</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C10,Etape1_CSV!$B$2:$B$1000,Etape1_CSV!$A$2:$A$1000),1)</f>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="10"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="8"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="10"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="8"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="10"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="8"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="8"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A15" s="10"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="8"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="H15" s="9"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A16" s="10"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="8"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="10"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="8"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
-      <c r="H17" s="9"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="10"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="8"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
-      <c r="H18" s="9"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1920705F-F5E0-9B44-9900-9A7C08A00BD3}">
+          <x14:formula1>
+            <xm:f>Lexique!$D$2:$D$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{07C27AF0-304E-B041-B524-3FD6C7C6F85F}">
+          <x14:formula1>
+            <xm:f>Lexique!$E$2:$E$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{783E0CD3-16A8-4440-9F89-CB4D8F2E4D16}">
+          <x14:formula1>
+            <xm:f>Lexique!$F$2:$F$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G10</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4800E175-391C-4882-AD71-91732BA4C7F2}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1960,38 +1790,34 @@
     <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
-        <v>136</v>
+      <c r="G1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -2001,23 +1827,19 @@
         <v>sign_01</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C2,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="str">
         <f>A2</f>
         <v>E2</v>
@@ -2030,23 +1852,19 @@
         <v>sign_02</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C3,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="str">
         <f t="shared" ref="A4:A18" si="1">A3</f>
         <v>E2</v>
@@ -2059,23 +1877,19 @@
         <v>sign_03</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C4,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" t="str">
         <f>A9</f>
         <v>E2</v>
@@ -2088,23 +1902,19 @@
         <v>sign_08</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C5,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" t="str">
         <f>A4</f>
         <v>E2</v>
@@ -2117,23 +1927,19 @@
         <v>sign_04</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C6,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2146,23 +1952,19 @@
         <v>sign_05</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C7,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>33.799999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2175,23 +1977,19 @@
         <v>sign_06</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C8,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>46.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2204,25 +2002,21 @@
         <v>sign_07</v>
       </c>
       <c r="D9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H9" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C9,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>54.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" t="str">
-        <f>A5</f>
+        <f t="shared" si="1"/>
         <v>E2</v>
       </c>
       <c r="B10" s="5">
@@ -2233,23 +2027,19 @@
         <v>sign_09</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
-      </c>
-      <c r="H10" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C10,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>75.099999999999994</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2262,23 +2052,19 @@
         <v>sign_10</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C11,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>77.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2291,23 +2077,19 @@
         <v>sign_11</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C12,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>87.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2320,23 +2102,19 @@
         <v>sign_12</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C13,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>89.2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2349,23 +2127,19 @@
         <v>sign_13</v>
       </c>
       <c r="D14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" t="s">
         <v>89</v>
       </c>
-      <c r="E14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" t="s">
-        <v>90</v>
-      </c>
       <c r="G14" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C14,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>112.7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2378,23 +2152,19 @@
         <v>sign_14</v>
       </c>
       <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
         <v>91</v>
       </c>
-      <c r="E15" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" t="s">
-        <v>92</v>
-      </c>
       <c r="G15" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C15,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>134.80000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2407,23 +2177,19 @@
         <v>sign_15</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G16" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C16,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>135.30000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2436,23 +2202,19 @@
         <v>sign_16</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G17" t="s">
-        <v>61</v>
-      </c>
-      <c r="H17" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C17,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>135.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" t="str">
         <f t="shared" si="1"/>
         <v>E2</v>
@@ -2465,20 +2227,16 @@
         <v>sign_17</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G18" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="9">
-        <f>ROUND(_xlfn.XLOOKUP(C18,Etape2_CSV!$B$2:$B$1000,Etape2_CSV!$A$2:$A$1000),1)</f>
-        <v>136.69999999999999</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2488,449 +2246,846 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{207A86C0-F1FC-5647-BA0D-4DE47D82F8C4}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB129F3F-5845-E94C-BB9B-41541692CC0D}">
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" customWidth="1"/>
-    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
-        <v>0</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="12">
-        <v>0.03</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
-        <v>0.98</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
-        <v>1.04</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="12">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="12">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="12">
-        <v>2.48</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="12">
-        <v>2.57</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="12">
-        <v>119.44</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>134</v>
-      </c>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <v>sign_01</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>A2</f>
+        <v>E3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f t="shared" ref="C3:C18" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <v>sign_02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A18" si="1">A3</f>
+        <v>E3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{43986E0E-F1BD-6B40-A89A-D1BF507D45E0}">
+          <x14:formula1>
+            <xm:f>Lexique!$D$2:$D$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CADB21EB-5FBA-F948-91A8-13DA27ECCDDC}">
+          <x14:formula1>
+            <xm:f>Lexique!$E$2:$E$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{446A4710-3B5A-9247-B67D-D204A01F91E2}">
+          <x14:formula1>
+            <xm:f>Lexique!$F$2:$F$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D5E8AE-63D3-48B9-85FC-50E5B76DED54}">
-  <dimension ref="A1:B39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F06BA10-C7CB-D34A-A68E-94110B0F7625}">
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>0.16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6">
-        <v>0.86</v>
-      </c>
-      <c r="B6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>0.96</v>
-      </c>
-      <c r="B7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>2.68</v>
-      </c>
-      <c r="B8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>4.04</v>
-      </c>
-      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>4.04</v>
-      </c>
-      <c r="B10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11">
-        <v>8.82</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A12">
-        <v>8.98</v>
-      </c>
-      <c r="B12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A14">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A15">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A16">
-        <v>33.82</v>
-      </c>
-      <c r="B16" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A17">
-        <v>44.88</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="E1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A18">
-        <v>46.16</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <v>sign_01</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A19">
-        <v>46.18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A20">
-        <v>54.64</v>
-      </c>
-      <c r="B20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A21">
-        <v>75.099999999999994</v>
-      </c>
-      <c r="B21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A22">
-        <v>77.459999999999994</v>
-      </c>
-      <c r="B22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A23">
-        <v>87.8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A24">
-        <v>87.8</v>
-      </c>
-      <c r="B24" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A25">
-        <v>89.05</v>
-      </c>
-      <c r="B25" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A26">
-        <v>89.23</v>
-      </c>
-      <c r="B26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A27">
-        <v>89.24</v>
-      </c>
-      <c r="B27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A28">
-        <v>112.65</v>
-      </c>
-      <c r="B28" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A29">
-        <v>134.77000000000001</v>
-      </c>
-      <c r="B29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A30">
-        <v>134.77000000000001</v>
-      </c>
-      <c r="B30" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A31">
-        <v>135.27000000000001</v>
-      </c>
-      <c r="B31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A32">
-        <v>135.44999999999999</v>
-      </c>
-      <c r="B32" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A33">
-        <v>135.46</v>
-      </c>
-      <c r="B33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A34">
-        <v>135.56</v>
-      </c>
-      <c r="B34" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A35">
-        <v>135.79</v>
-      </c>
-      <c r="B35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A36">
-        <v>136.19</v>
-      </c>
-      <c r="B36" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A37">
-        <v>136.37</v>
-      </c>
-      <c r="B37" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A38">
-        <v>136.69999999999999</v>
-      </c>
-      <c r="B38" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A39">
-        <v>136.71</v>
-      </c>
-      <c r="B39" t="s">
-        <v>134</v>
-      </c>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>A2</f>
+        <v>E3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f t="shared" ref="C3:C18" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <v>sign_02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4" si="1">A3</f>
+        <v>E3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6CAFD195-8F48-7146-8CCC-7F3285E5E5C3}">
+          <x14:formula1>
+            <xm:f>Lexique!$F$2:$F$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B0DF1CBE-BD5F-4748-ABA8-9AE21064C1D2}">
+          <x14:formula1>
+            <xm:f>Lexique!$E$2:$E$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E6622F3-25B6-4E48-B957-A1F985497D26}">
+          <x14:formula1>
+            <xm:f>Lexique!$D$2:$D$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD59B0A2-43B3-4B44-B4E7-3010D763E1BD}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <v>sign_01</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>A2</f>
+        <v>E3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f t="shared" ref="C3:C18" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <v>sign_02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4" si="1">A3</f>
+        <v>E3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{062F1F6B-EF2B-1542-84B0-5A0FFF18622E}">
+          <x14:formula1>
+            <xm:f>Lexique!$F$2:$F$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0F630894-249D-C244-99EB-56CB5D569155}">
+          <x14:formula1>
+            <xm:f>Lexique!$E$2:$E$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EEFC1E61-00EB-A04F-89A9-AA3E02490524}">
+          <x14:formula1>
+            <xm:f>Lexique!$D$2:$D$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA1B73-E162-C44F-BFAF-F0B7401711F0}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <v>sign_01</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>A2</f>
+        <v>E3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f t="shared" ref="C3:C18" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <v>sign_02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4" si="1">A3</f>
+        <v>E3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CA9A1E28-3F62-C242-BCBA-BAFF06DAB59D}">
+          <x14:formula1>
+            <xm:f>Lexique!$D$2:$D$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1B1D86AE-4853-1B43-B675-11AA20C5B33C}">
+          <x14:formula1>
+            <xm:f>Lexique!$E$2:$E$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{698F6BB2-A1D9-3B48-8632-9499230BEEEB}">
+          <x14:formula1>
+            <xm:f>Lexique!$F$2:$F$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F8F1C6-7AEF-9949-BBA2-37380A45C53E}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="5">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <v>sign_01</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>A2</f>
+        <v>E3</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f t="shared" ref="C3:C18" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <v>sign_02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4" si="1">A3</f>
+        <v>E3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{45B62D04-6757-7944-9BE6-89C95E9DC451}">
+          <x14:formula1>
+            <xm:f>Lexique!$F$2:$F$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3D343D7E-CDE1-3A43-9638-EA1D8860F6B1}">
+          <x14:formula1>
+            <xm:f>Lexique!$E$2:$E$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B85CEF8C-511F-3C46-A27A-714B22416C96}">
+          <x14:formula1>
+            <xm:f>Lexique!$D$2:$D$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout sign etape 6, ref #41
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8AA49E4-ADFB-7A4B-8AEE-1CC49B3BFF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E4D11E-220E-5C49-BC96-BE4B90F49F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22160" yWindow="4960" windowWidth="40640" windowHeight="21000" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="102460" yWindow="4240" windowWidth="33480" windowHeight="20380" tabRatio="758" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="190">
   <si>
     <t>GPM</t>
   </si>
@@ -584,6 +584,66 @@
   </si>
   <si>
     <t>Déviation des voitures équipe suiveuse - 3e &amp; 1ere</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>Contrôle policier. Gestion de l'intersection route 109 et route 395</t>
+  </si>
+  <si>
+    <t>Pont de bois à la rivière Kinojevis</t>
+  </si>
+  <si>
+    <t>Terre plein à la première sortie du rond point toute à gauche</t>
+  </si>
+  <si>
+    <t>Terre plein, toute à la gauche (Devant Plomberie Germain Roy)</t>
+  </si>
+  <si>
+    <t>Terre plein, toute à la gauche (Devant Mill Vitres d'Autos)</t>
+  </si>
+  <si>
+    <t>Terre plein, toute à la gauche (Devant Cordonnerie M Paquin)</t>
+  </si>
+  <si>
+    <t>Terre plein, toute à la gauche (Devant Thibault Chrysler)</t>
+  </si>
+  <si>
+    <t>Terre plein, toute à la gauche (Devant l'Oasis)</t>
+  </si>
+  <si>
+    <t>Terre plein, toute à la gauche (Devant Accent Plein-Air)</t>
+  </si>
+  <si>
+    <t>Terre plein, toute à la gauche (Devant cinéma Amos)</t>
+  </si>
+  <si>
+    <t>Terre plein, toute à la gauche (Devant Shell)</t>
+  </si>
+  <si>
+    <t>Voie ferrée perpendiculaire à la route</t>
+  </si>
+  <si>
+    <t>Contrôle policier. Intersection route 109 / rue principal RH. Rester à droite bretelle vers Rouyn</t>
+  </si>
+  <si>
+    <t>Contrôle policier. Intersection route 109 / route 117 RH</t>
+  </si>
+  <si>
+    <t>Rond point.Tout à gauche du terre-plein en sens inverse de la circulation - Moto et police</t>
+  </si>
+  <si>
+    <t>Avancée de trottoir devant McDo à protéger (cônes) et signaler</t>
+  </si>
+  <si>
+    <t>Passage rond-point en neutralisé, gestion policière</t>
+  </si>
+  <si>
+    <t>Contrôle policier. Gestion du virage à droite vers route 395, bretelle vers Preissac</t>
+  </si>
+  <si>
+    <t>Contrôle policier, intersection 111/109</t>
   </si>
 </sst>
 </file>
@@ -677,7 +737,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -709,12 +769,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -729,6 +802,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1328,7 +1404,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1642,7 +1718,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2244,7 +2320,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U35" sqref="U35"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2601,8 +2677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB129F3F-5845-E94C-BB9B-41541692CC0D}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2659,8 +2735,8 @@
       <c r="F2" t="s">
         <v>77</v>
       </c>
-      <c r="G2" t="s">
-        <v>67</v>
+      <c r="G2" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -2690,7 +2766,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="str">
-        <f t="shared" ref="A4:A12" si="1">A3</f>
+        <f t="shared" ref="A4:A10" si="1">A3</f>
         <v>E3</v>
       </c>
       <c r="B4" s="5">
@@ -2917,7 +2993,7 @@
           <x14:formula1>
             <xm:f>Lexique!$F$2:$F$13</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G10</xm:sqref>
+          <xm:sqref>G3:G10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3099,7 +3175,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3265,19 +3341,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA1B73-E162-C44F-BFAF-F0B7401711F0}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="62.5" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="83.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -3307,9 +3383,9 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="5">
+        <v>170</v>
+      </c>
+      <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="str">
@@ -3317,114 +3393,527 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>102</v>
+        <v>171</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" t="str">
         <f>A2</f>
-        <v>E3</v>
-      </c>
-      <c r="B3" s="5">
+        <v>E6</v>
+      </c>
+      <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="str">
-        <f t="shared" ref="C3:C4" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <f t="shared" ref="C3:C20" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
         <v>sign_02</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" t="str">
-        <f t="shared" ref="A4" si="1">A3</f>
-        <v>E3</v>
-      </c>
-      <c r="B4" s="5">
+        <f t="shared" ref="A4:A28" si="1">A3</f>
+        <v>E6</v>
+      </c>
+      <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="str">
         <f t="shared" si="0"/>
         <v>sign_03</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_04</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="A6" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_05</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_06</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_07</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_08</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_09</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="A13" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_12</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="A15" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="A16" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_15</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_16</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_17</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B19" s="2">
+        <v>50</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_50</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>51</v>
+      </c>
+      <c r="C20" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_51</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CA9A1E28-3F62-C242-BCBA-BAFF06DAB59D}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{70C67CA6-BE58-AD46-83A8-E5FA73FBD4BB}">
           <x14:formula1>
-            <xm:f>Lexique!$D$2:$D$10</xm:f>
+            <xm:f>Lexique!$F$2:$F$17</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1B1D86AE-4853-1B43-B675-11AA20C5B33C}">
-          <x14:formula1>
-            <xm:f>Lexique!$E$2:$E$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{698F6BB2-A1D9-3B48-8632-9499230BEEEB}">
-          <x14:formula1>
-            <xm:f>Lexique!$F$2:$F$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G8</xm:sqref>
+          <xm:sqref>G2:G18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Corrections et compilation Etape 5, ref #47
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4486F0-1421-0446-8A3A-21D3FE98951A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E75D84-B8FF-674C-BE5D-8D022C86066C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="204">
   <si>
     <t>GPM</t>
   </si>
@@ -683,6 +683,9 @@
   </si>
   <si>
     <t>Déviation caravane - sortie véhicules support</t>
+  </si>
+  <si>
+    <t>sign_60</t>
   </si>
 </sst>
 </file>
@@ -3182,7 +3185,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3710,7 +3713,7 @@
         <v>60</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>202</v>

</xml_diff>

<commit_message>
Ajout images et description signalisation, ref #48
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E75D84-B8FF-674C-BE5D-8D022C86066C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927947B4-3B11-4D46-8A7A-9818EF5BC71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50880" yWindow="2480" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="219">
   <si>
     <t>GPM</t>
   </si>
@@ -382,9 +382,6 @@
     <t>E3</t>
   </si>
   <si>
-    <t>Description 1</t>
-  </si>
-  <si>
     <t>-------------------</t>
   </si>
   <si>
@@ -686,6 +683,54 @@
   </si>
   <si>
     <t>sign_60</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>Entrée rond-point du ch. Camping - Neutralisé</t>
+  </si>
+  <si>
+    <t>Gestion circulation rond-point</t>
+  </si>
+  <si>
+    <t>Légèrement à gauche - Ch Lac Mourier</t>
+  </si>
+  <si>
+    <t>Légèrement à gauche - Rivière-Héva &amp; Intersection Amos</t>
+  </si>
+  <si>
+    <t>Point de croisement de la course - Cadillac</t>
+  </si>
+  <si>
+    <t>Contrôle Traffic 117</t>
+  </si>
+  <si>
+    <t>Bollards vidange roulottes - signalisation pour protéger - Ville de RN</t>
+  </si>
+  <si>
+    <t>Rétrécicement troittoir - signalisation pour protéger - Ville de RN</t>
+  </si>
+  <si>
+    <t>Virage gauche - Bureau de Poste</t>
+  </si>
+  <si>
+    <t>Virage droite - retour 117 -- Danger Croisement</t>
+  </si>
+  <si>
+    <t>Entrée rond-point Malartic - Toute à droite</t>
+  </si>
+  <si>
+    <t>Gestion dans rond-point - Signaleur et SQ pour traffic</t>
+  </si>
+  <si>
+    <t>Virage gauche - Harricana</t>
+  </si>
+  <si>
+    <t>Virage gauche - 4e avenue</t>
+  </si>
+  <si>
+    <t>Déviation caravane - des Érables</t>
   </si>
 </sst>
 </file>
@@ -1387,7 +1432,7 @@
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
@@ -1397,7 +1442,7 @@
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1467,7 +1512,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
@@ -1507,7 +1552,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -1530,7 +1575,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>56</v>
@@ -1555,7 +1600,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
@@ -1583,7 +1628,7 @@
         <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>5</v>
@@ -1671,7 +1716,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C18" t="s">
         <v>44</v>
@@ -1690,13 +1735,13 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
@@ -1773,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>95</v>
@@ -1796,7 +1841,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>96</v>
@@ -1819,7 +1864,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>97</v>
@@ -1842,7 +1887,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>98</v>
@@ -1865,7 +1910,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D6" t="s">
         <v>75</v>
@@ -1888,7 +1933,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D7" t="s">
         <v>85</v>
@@ -1911,7 +1956,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
         <v>86</v>
@@ -1934,7 +1979,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
         <v>87</v>
@@ -1957,7 +2002,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D10" t="s">
         <v>88</v>
@@ -1980,10 +2025,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" t="s">
         <v>140</v>
-      </c>
-      <c r="D11" t="s">
-        <v>141</v>
       </c>
       <c r="E11" t="s">
         <v>56</v>
@@ -2003,10 +2048,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" t="s">
         <v>142</v>
-      </c>
-      <c r="D12" t="s">
-        <v>143</v>
       </c>
       <c r="E12" t="s">
         <v>56</v>
@@ -2026,10 +2071,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E13" t="s">
         <v>56</v>
@@ -2049,10 +2094,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E14" t="s">
         <v>56</v>
@@ -2072,10 +2117,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E15" t="s">
         <v>56</v>
@@ -2095,10 +2140,10 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" t="s">
         <v>147</v>
-      </c>
-      <c r="D16" t="s">
-        <v>148</v>
       </c>
       <c r="E16" t="s">
         <v>64</v>
@@ -2118,10 +2163,10 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E17" t="s">
         <v>64</v>
@@ -2141,10 +2186,10 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E18" t="s">
         <v>64</v>
@@ -2164,10 +2209,10 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E19" t="s">
         <v>64</v>
@@ -2187,10 +2232,10 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E20" t="s">
         <v>64</v>
@@ -2210,10 +2255,10 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
@@ -2233,10 +2278,10 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E22" t="s">
         <v>64</v>
@@ -2256,7 +2301,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D23" t="s">
         <v>75</v>
@@ -2279,10 +2324,10 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" t="s">
         <v>153</v>
-      </c>
-      <c r="D24" t="s">
-        <v>154</v>
       </c>
       <c r="E24" t="s">
         <v>56</v>
@@ -2375,7 +2420,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
@@ -2398,7 +2443,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
         <v>71</v>
@@ -2421,7 +2466,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
         <v>73</v>
@@ -2444,7 +2489,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
         <v>75</v>
@@ -2467,10 +2512,10 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s">
         <v>114</v>
-      </c>
-      <c r="D6" t="s">
-        <v>115</v>
       </c>
       <c r="E6" t="s">
         <v>64</v>
@@ -2490,10 +2535,10 @@
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" t="s">
         <v>64</v>
@@ -2513,7 +2558,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
         <v>76</v>
@@ -2536,7 +2581,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D9" t="s">
         <v>78</v>
@@ -2559,7 +2604,7 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
         <v>80</v>
@@ -2582,7 +2627,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
         <v>81</v>
@@ -2605,7 +2650,7 @@
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D12" t="s">
         <v>82</v>
@@ -2737,7 +2782,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E2" t="s">
         <v>65</v>
@@ -2762,7 +2807,7 @@
         <v>sign_02</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
         <v>65</v>
@@ -2787,7 +2832,7 @@
         <v>sign_03</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E4" t="s">
         <v>64</v>
@@ -2812,7 +2857,7 @@
         <v>sign_50</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -2837,7 +2882,7 @@
         <v>sign_60</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E6" t="s">
         <v>64</v>
@@ -2862,7 +2907,7 @@
         <v>sign_70</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E7" t="s">
         <v>64</v>
@@ -2887,7 +2932,7 @@
         <v>sign_90</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E8" t="s">
         <v>65</v>
@@ -2912,7 +2957,7 @@
         <v>sign_91</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -2937,7 +2982,7 @@
         <v>sign_92</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
@@ -3015,8 +3060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F06BA10-C7CB-D34A-A68E-94110B0F7625}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3025,9 +3070,7 @@
     <col min="2" max="2" width="2.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="62.5" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -3054,93 +3097,349 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="5">
+      <c r="A2" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
-        <v>sign_01</v>
+      <c r="C2" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>102</v>
+        <v>204</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" t="str">
-        <f>A2</f>
-        <v>E3</v>
-      </c>
-      <c r="B3" s="5">
+      <c r="A3" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="str">
-        <f t="shared" ref="C3:C4" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
-        <v>sign_02</v>
+      <c r="C3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" t="str">
-        <f t="shared" ref="A4" si="1">A3</f>
-        <v>E3</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="A4" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>sign_03</v>
+      <c r="C4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="A6" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="A7" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="A8" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="A9" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="A10" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="A11" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="A13" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="A15" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B17" s="5"/>
@@ -3153,30 +3452,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6CAFD195-8F48-7146-8CCC-7F3285E5E5C3}">
-          <x14:formula1>
-            <xm:f>Lexique!$F$2:$F$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B0DF1CBE-BD5F-4748-ABA8-9AE21064C1D2}">
-          <x14:formula1>
-            <xm:f>Lexique!$E$2:$E$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2E6622F3-25B6-4E48-B957-A1F985497D26}">
-          <x14:formula1>
-            <xm:f>Lexique!$D$2:$D$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E4</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3184,7 +3459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD59B0A2-43B3-4B44-B4E7-3010D763E1BD}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -3224,16 +3499,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
@@ -3247,16 +3522,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>56</v>
@@ -3270,16 +3545,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>64</v>
@@ -3293,13 +3568,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>88</v>
@@ -3316,13 +3591,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>87</v>
@@ -3339,13 +3614,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>86</v>
@@ -3362,13 +3637,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>85</v>
@@ -3385,13 +3660,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>75</v>
@@ -3408,16 +3683,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>56</v>
@@ -3431,16 +3706,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>65</v>
@@ -3449,21 +3724,21 @@
         <v>77</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>65</v>
@@ -3472,21 +3747,21 @@
         <v>77</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>64</v>
@@ -3500,13 +3775,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14" s="2">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>75</v>
@@ -3523,16 +3798,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B15" s="2">
         <v>14</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>64</v>
@@ -3546,16 +3821,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B16" s="2">
         <v>15</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>64</v>
@@ -3569,16 +3844,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B17" s="2">
         <v>16</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>64</v>
@@ -3592,16 +3867,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>64</v>
@@ -3615,16 +3890,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B19" s="2">
         <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>64</v>
@@ -3638,16 +3913,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B20" s="2">
         <v>19</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>64</v>
@@ -3661,16 +3936,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B21" s="2">
         <v>50</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>64</v>
@@ -3684,16 +3959,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B22" s="2">
         <v>51</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>64</v>
@@ -3707,16 +3982,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B23" s="2">
         <v>60</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>56</v>
@@ -3778,7 +4053,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -3788,7 +4063,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>64</v>
@@ -3813,7 +4088,7 @@
         <v>sign_02</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>64</v>
@@ -3838,7 +4113,7 @@
         <v>sign_03</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>64</v>
@@ -3863,7 +4138,7 @@
         <v>sign_04</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>64</v>
@@ -3888,7 +4163,7 @@
         <v>sign_05</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>56</v>
@@ -3913,7 +4188,7 @@
         <v>sign_06</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>64</v>
@@ -3938,7 +4213,7 @@
         <v>sign_07</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>64</v>
@@ -3963,7 +4238,7 @@
         <v>sign_08</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>64</v>
@@ -3988,7 +4263,7 @@
         <v>sign_09</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>64</v>
@@ -4013,7 +4288,7 @@
         <v>sign_10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>64</v>
@@ -4038,7 +4313,7 @@
         <v>sign_11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>64</v>
@@ -4063,7 +4338,7 @@
         <v>sign_12</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>64</v>
@@ -4088,7 +4363,7 @@
         <v>sign_13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>64</v>
@@ -4113,7 +4388,7 @@
         <v>sign_14</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>64</v>
@@ -4138,7 +4413,7 @@
         <v>sign_15</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>64</v>
@@ -4163,7 +4438,7 @@
         <v>sign_16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>65</v>
@@ -4188,7 +4463,7 @@
         <v>sign_17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>64</v>
@@ -4213,7 +4488,7 @@
         <v>sign_50</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>64</v>
@@ -4238,7 +4513,7 @@
         <v>sign_51</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>64</v>
@@ -4360,7 +4635,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -4370,7 +4645,7 @@
         <v>sign_01</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E2" t="s">
         <v>64</v>
@@ -4395,7 +4670,7 @@
         <v>sign_02</v>
       </c>
       <c r="D3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" t="s">
         <v>64</v>
@@ -4420,7 +4695,7 @@
         <v>sign_03</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
         <v>64</v>
@@ -4445,7 +4720,7 @@
         <v>sign_04</v>
       </c>
       <c r="D5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E5" t="s">
         <v>64</v>
@@ -4470,7 +4745,7 @@
         <v>sign_05</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" t="s">
         <v>64</v>
@@ -4495,7 +4770,7 @@
         <v>sign_06</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
         <v>64</v>
@@ -4520,7 +4795,7 @@
         <v>sign_07</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
         <v>56</v>
@@ -4545,7 +4820,7 @@
         <v>sign_08</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
@@ -4570,7 +4845,7 @@
         <v>sign_09</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
         <v>56</v>
@@ -4595,7 +4870,7 @@
         <v>sign_10</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" t="s">
         <v>56</v>
@@ -4645,7 +4920,7 @@
         <v>sign_12</v>
       </c>
       <c r="D13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E13" t="s">
         <v>56</v>
@@ -4720,7 +4995,7 @@
         <v>sign_15</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E16" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Nouvelles images sign E5
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr date1904="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927947B4-3B11-4D46-8A7A-9818EF5BC71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB395740-2BE7-FC43-B5ED-C9F98F6452BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50880" yWindow="2480" windowWidth="33600" windowHeight="20500" tabRatio="758" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="102460" yWindow="4240" windowWidth="33480" windowHeight="20380" tabRatio="758" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="Etape2" sheetId="26" r:id="rId4"/>
     <sheet name="Etape3" sheetId="31" r:id="rId5"/>
     <sheet name="Etape4" sheetId="32" r:id="rId6"/>
-    <sheet name="Etape5" sheetId="33" r:id="rId7"/>
+    <sheet name="Etape5" sheetId="36" r:id="rId7"/>
     <sheet name="Etape6" sheetId="34" r:id="rId8"/>
     <sheet name="Etape7" sheetId="35" r:id="rId9"/>
+    <sheet name="Etape5_Senneterre_Annulee" sheetId="33" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="224">
   <si>
     <t>GPM</t>
   </si>
@@ -731,6 +732,21 @@
   </si>
   <si>
     <t>Déviation caravane - des Érables</t>
+  </si>
+  <si>
+    <t>Contrôle policier. Intersection route 109 / rue principal RH. Tout droit vers St-Mathieu</t>
+  </si>
+  <si>
+    <t>Bretelle vers 117, tout à gauche (sens inverse)</t>
+  </si>
+  <si>
+    <t>Bretelle vers rue Quatre-Coin RH (sens normal circulation)</t>
+  </si>
+  <si>
+    <t>Contrôle policier. Gestion du virage à droite vers route 395, bretelle de Preissac</t>
+  </si>
+  <si>
+    <t>Contrôle policier. Gestion de l'intersection route 109 et route 111/395</t>
   </si>
 </sst>
 </file>
@@ -799,7 +815,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -821,6 +837,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFDE9D9"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -874,7 +896,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -891,6 +913,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -1451,6 +1477,560 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD59B0A2-43B3-4B44-B4E7-3010D763E1BD}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="62.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" s="2">
+        <v>50</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="2">
+        <v>51</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B23" s="2">
+        <v>60</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31D78861-6A86-448A-A85A-2A1E287D1373}">
   <dimension ref="A1:F21"/>
@@ -3060,7 +3640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F06BA10-C7CB-D34A-A68E-94110B0F7625}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
@@ -3456,11 +4036,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD59B0A2-43B3-4B44-B4E7-3010D763E1BD}">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308A417D-3276-6C45-809F-C6AB563D40A7}">
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3468,8 +4048,8 @@
     <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="62.5" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="83.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1640625" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -3498,270 +4078,293 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="13" t="s">
-        <v>189</v>
+      <c r="A2" t="str">
+        <f>A22</f>
+        <v>E6</v>
       </c>
       <c r="B2" s="2">
+        <v>50</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B2,"0#"))</f>
+        <v>sign_50</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" t="str">
+        <f>A2</f>
+        <v>E6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>51</v>
+      </c>
+      <c r="C3" s="14" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B3,"0#"))</f>
+        <v>sign_51</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" t="str">
+        <f>A6</f>
+        <v>E6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5</v>
+      </c>
+      <c r="C4" s="14" t="str">
+        <f t="shared" ref="C4:C22" si="0">_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B4,"0#"))</f>
+        <v>sign_05</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" t="str">
+        <f t="shared" ref="A5:A30" si="1">A4</f>
+        <v>E6</v>
+      </c>
+      <c r="B5">
+        <v>61</v>
+      </c>
+      <c r="C5" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_61</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" t="str">
+        <f>A8</f>
+        <v>E6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="17" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B6,"0#"))</f>
+        <v>sign_04</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" t="str">
+        <f>A5</f>
+        <v>E6</v>
+      </c>
+      <c r="B7">
+        <v>62</v>
+      </c>
+      <c r="C7" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_62</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" t="str">
+        <f>A9</f>
+        <v>E6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="17" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B8,"0#"))</f>
+        <v>sign_03</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" t="str">
+        <f>A10</f>
+        <v>E6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="17" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B9,"0#"))</f>
+        <v>sign_02</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B4" s="2">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="C10" s="17" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"sign",TEXT(B10,"0#"))</f>
+        <v>sign_01</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" t="str">
+        <f>A4</f>
+        <v>E6</v>
+      </c>
+      <c r="B11" s="2">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_06</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B12" s="2">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_07</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B7" s="2">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B8" s="2">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="G12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B13" s="2">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B10" s="2">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B11" s="2">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B12" s="2">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B13" s="2">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>115</v>
+      <c r="C13" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_08</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>64</v>
@@ -3769,45 +4372,49 @@
       <c r="F13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>74</v>
+      <c r="G13" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
-        <v>189</v>
+      <c r="A14" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
       </c>
       <c r="B14" s="2">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>108</v>
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_09</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>75</v>
+        <v>174</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
-        <v>189</v>
+      <c r="A15" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
       </c>
       <c r="B15" s="2">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>109</v>
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>64</v>
@@ -3815,197 +4422,248 @@
       <c r="F15" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>74</v>
+      <c r="G15" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>189</v>
+      <c r="A16" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
       </c>
       <c r="B16" s="2">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_11</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B17" s="2">
+        <v>12</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_12</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B18" s="2">
+        <v>13</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_13</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B19" s="2">
+        <v>14</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_14</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B20" s="2">
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="C20" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_15</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B21" s="2">
         <v>16</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B18" s="2">
+      <c r="C21" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_16</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+      <c r="B22" s="2">
         <v>17</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B19" s="2">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B20" s="2">
-        <v>19</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B21" s="2">
-        <v>50</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B22" s="2">
-        <v>51</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>199</v>
+      <c r="C22" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>sign_17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>64</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
+      </c>
+      <c r="G22" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B23" s="2">
-        <v>60</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>56</v>
+      <c r="A23" t="str">
+        <f>A3</f>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" t="str">
+        <f>A28</f>
+        <v>E6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" t="str">
+        <f t="shared" si="1"/>
+        <v>E6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A09A0CE1-1AC3-904E-B54E-B2920560C3D7}">
+          <x14:formula1>
+            <xm:f>Lexique!$F$2:$F$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G22 G10</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Ajout POI Poularie pour moto
</commit_message>
<xml_diff>
--- a/excel/signalisation.xlsx
+++ b/excel/signalisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79761C3B-21EA-8D40-BCC6-602C75C092E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6146ADB2-DA0A-8D41-9CB1-57883A71DE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="102460" yWindow="4240" windowWidth="33480" windowHeight="20380" tabRatio="758" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="102460" yWindow="4240" windowWidth="33480" windowHeight="20380" tabRatio="758" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="23" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="225">
   <si>
     <t>GPM</t>
   </si>
@@ -747,6 +747,9 @@
   </si>
   <si>
     <t>Contrôle policier. Gestion de l'intersection route 109 et route 111/395</t>
+  </si>
+  <si>
+    <t>Virage à droite sur route 390</t>
   </si>
 </sst>
 </file>
@@ -2953,8 +2956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4800E175-391C-4882-AD71-91732BA4C7F2}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3110,46 +3113,46 @@
       <c r="A7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>114</v>
       </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="11" t="s">
+      <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="11" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E8" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
@@ -3157,22 +3160,22 @@
         <v>84</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
@@ -3180,22 +3183,22 @@
         <v>84</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E10" t="s">
         <v>64</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
@@ -3203,22 +3206,22 @@
         <v>84</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
         <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -3226,27 +3229,46 @@
         <v>84</v>
       </c>
       <c r="B12">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>112</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>82</v>
       </c>
-      <c r="E12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
         <v>77</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B14" s="5"/>
@@ -3287,19 +3309,19 @@
           <x14:formula1>
             <xm:f>Lexique!$D$2:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>E14:E1048576 E2:E13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8B2F24BC-BBE5-3242-8C11-39321438202A}">
           <x14:formula1>
             <xm:f>Lexique!$E$2:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>F14:F1048576 F2:F13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2AB93EB3-1866-E243-98C3-B11D12762F37}">
           <x14:formula1>
             <xm:f>Lexique!$F$2:$F$17</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
+          <xm:sqref>G14:G1048576 G2:G13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4038,7 +4060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{308A417D-3276-6C45-809F-C6AB563D40A7}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>

</xml_diff>